<commit_message>
Updated the Excel files for the first 4 centers so that the markers are more straightforward to parse.
</commit_message>
<xml_diff>
--- a/Miami.xlsx
+++ b/Miami.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Comp controls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="99">
   <si>
     <t>Marker</t>
   </si>
@@ -64,21 +64,9 @@
     <t>T, B, DC/mono/NK, Th1/2/17</t>
   </si>
   <si>
-    <t>CD127 Alexa 647</t>
-  </si>
-  <si>
-    <t>CD8 APC-H7</t>
-  </si>
-  <si>
-    <t>CD45RO APC-H7</t>
-  </si>
-  <si>
     <t>T cell, Th1/2/17</t>
   </si>
   <si>
-    <t>CD3+19+20 APC-H7</t>
-  </si>
-  <si>
     <t>PLEASE FILL IN THE YELLOW SHADED CELLS:</t>
   </si>
   <si>
@@ -148,30 +136,6 @@
     <t>Compensation Controls_HLA-DR AmCyan Stained Control_G05.fcs</t>
   </si>
   <si>
-    <t>FITC</t>
-  </si>
-  <si>
-    <t>PE-A</t>
-  </si>
-  <si>
-    <t>PerCP-Cy5-5-A</t>
-  </si>
-  <si>
-    <t>APC-A</t>
-  </si>
-  <si>
-    <t>APC-Cy7-A</t>
-  </si>
-  <si>
-    <t>Pacific Blue-A</t>
-  </si>
-  <si>
-    <t>AmCyan-A</t>
-  </si>
-  <si>
-    <t>PE Cy7</t>
-  </si>
-  <si>
     <t>lot 12828_A1_A01.fcs</t>
   </si>
   <si>
@@ -305,6 +269,54 @@
   </si>
   <si>
     <t>lot 1369_E9_E09.fcs</t>
+  </si>
+  <si>
+    <t>LIVE GREEN:FITC</t>
+  </si>
+  <si>
+    <t>CD197:PE-A</t>
+  </si>
+  <si>
+    <t>CD4:PerCP-Cy5-5-A</t>
+  </si>
+  <si>
+    <t>CD45RA:PE Cy7</t>
+  </si>
+  <si>
+    <t>CD194:PE Cy7</t>
+  </si>
+  <si>
+    <t>CD27:PE Cy7</t>
+  </si>
+  <si>
+    <t>CD11c:PE Cy7</t>
+  </si>
+  <si>
+    <t>CD196:PE Cy7</t>
+  </si>
+  <si>
+    <t>CD38:APC-A</t>
+  </si>
+  <si>
+    <t>CD127:Alexa 647</t>
+  </si>
+  <si>
+    <t>CD8:APC-H7</t>
+  </si>
+  <si>
+    <t>CD45RO:APC-H7</t>
+  </si>
+  <si>
+    <t>CD20:APC-Cy7-A</t>
+  </si>
+  <si>
+    <t>CD3+19+20:APC-H7</t>
+  </si>
+  <si>
+    <t>CD3:Pacific Blue-A</t>
+  </si>
+  <si>
+    <t>HLA-DR:AmCyan-A</t>
   </si>
 </sst>
 </file>
@@ -317,6 +329,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -808,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -823,7 +836,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -843,7 +856,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -866,10 +879,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -889,10 +902,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -912,10 +925,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -935,10 +948,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -958,10 +971,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -981,10 +994,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -1004,10 +1017,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1027,10 +1040,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1050,10 +1063,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -1073,10 +1086,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -1096,13 +1109,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3">
         <v>22500</v>
@@ -1119,10 +1132,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -1142,10 +1155,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1165,10 +1178,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1188,10 +1201,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1211,10 +1224,10 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1247,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="H15" sqref="H14:H15"/>
     </sheetView>
   </sheetViews>
@@ -1261,32 +1274,32 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1300,7 +1313,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" t="s">
@@ -1315,7 +1328,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" t="s">
@@ -1330,7 +1343,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" t="s">
@@ -1345,7 +1358,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" t="s">
@@ -1360,7 +1373,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" t="s">
@@ -1375,7 +1388,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" t="s">
@@ -1390,7 +1403,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" t="s">
@@ -1405,7 +1418,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" t="s">
@@ -1420,7 +1433,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" t="s">
@@ -1435,7 +1448,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" t="s">
@@ -1450,7 +1463,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" t="s">
@@ -1465,7 +1478,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" t="s">
@@ -1480,7 +1493,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" t="s">
@@ -1495,7 +1508,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" t="s">
@@ -1510,7 +1523,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" t="s">
@@ -1525,7 +1538,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" t="s">
@@ -1540,7 +1553,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" t="s">
@@ -1555,7 +1568,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" t="s">
@@ -1570,7 +1583,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" t="s">
@@ -1585,7 +1598,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" t="s">
@@ -1600,7 +1613,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" t="s">
@@ -1615,7 +1628,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" t="s">
@@ -1630,7 +1643,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" t="s">
@@ -1645,7 +1658,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" t="s">
@@ -1660,7 +1673,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" t="s">
@@ -1675,7 +1688,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" t="s">
@@ -1690,7 +1703,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" t="s">
@@ -1705,7 +1718,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" t="s">
@@ -1720,7 +1733,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" t="s">
@@ -1735,7 +1748,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" t="s">
@@ -1750,7 +1763,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" t="s">
@@ -1765,7 +1778,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" t="s">
@@ -1780,7 +1793,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" t="s">
@@ -1795,7 +1808,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" t="s">
@@ -1810,7 +1823,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" t="s">
@@ -1825,7 +1838,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" t="s">
@@ -1840,7 +1853,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" t="s">
@@ -1855,7 +1868,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" t="s">
@@ -1870,7 +1883,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" t="s">
@@ -1885,7 +1898,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" t="s">
@@ -1900,7 +1913,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" t="s">
@@ -1915,7 +1928,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" t="s">
@@ -1930,7 +1943,7 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" t="s">
@@ -1945,7 +1958,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" t="s">

</xml_diff>